<commit_message>
Added new testCase for account creation
</commit_message>
<xml_diff>
--- a/MyStoreProject/src/test/resources/TestData/TestData.xlsx
+++ b/MyStoreProject/src/test/resources/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Email" sheetId="3" r:id="rId3"/>
     <sheet name="ProductDetails" sheetId="4" r:id="rId4"/>
     <sheet name="SearchProduct" sheetId="6" r:id="rId5"/>
+    <sheet name="AccountCreationData" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="88">
   <si>
     <t>TestCases</t>
   </si>
@@ -200,6 +201,93 @@
   </si>
   <si>
     <t>ghfsdtyfg@gmail.com</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>SetPassword</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zipcode</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>MobilePhone</t>
+  </si>
+  <si>
+    <t>Mrs</t>
+  </si>
+  <si>
+    <t>hgsdhj</t>
+  </si>
+  <si>
+    <t>jhgfdsuy</t>
+  </si>
+  <si>
+    <t>hgsdtyf</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>1985</t>
+  </si>
+  <si>
+    <t>hjgsy</t>
+  </si>
+  <si>
+    <t>EDFG123</t>
+  </si>
+  <si>
+    <t>San</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>91436</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>8489875678</t>
+  </si>
+  <si>
+    <t>teshgdfg@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -329,7 +417,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -360,6 +448,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -960,9 +1050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1046,4 +1134,133 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated data provider method for createAccountTest
</commit_message>
<xml_diff>
--- a/MyStoreProject/src/test/resources/TestData/TestData.xlsx
+++ b/MyStoreProject/src/test/resources/TestData/TestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="90">
   <si>
     <t>TestCases</t>
   </si>
@@ -287,7 +287,13 @@
     <t>ABCDEF</t>
   </si>
   <si>
-    <t>hjgftrgfhgt@gmail.com</t>
+    <t>newtest1@gmail.com</t>
+  </si>
+  <si>
+    <t>newtest2@gmail.com</t>
+  </si>
+  <si>
+    <t>newtest3@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1138,9 +1144,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1255,9 +1263,105 @@
         <v>83</v>
       </c>
     </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>